<commit_message>
Created the design for about page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,6 +714,29 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>jameel khan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>jameela@gmail.com</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>9654879897</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>